<commit_message>
Penambahan satu fungsi data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding Stuff\Github\Visualisasi-Prediksi-Pengangguran-Terbuka-Berdasarkan-Umur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3A7753-59CC-4AB2-90E0-EFC0D9CFE09A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C819DF87-4232-4FC5-BFBF-27F6C5FB378A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{B7CE34E8-073A-42E5-8AA2-11B12B6674C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="6" xr2:uid="{B7CE34E8-073A-42E5-8AA2-11B12B6674C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Before" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Data Training" sheetId="5" r:id="rId4"/>
     <sheet name="Data Testing" sheetId="6" r:id="rId5"/>
     <sheet name="Data" sheetId="7" r:id="rId6"/>
-    <sheet name="Testing" sheetId="8" r:id="rId7"/>
+    <sheet name="Ramalan" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -438,6 +438,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -449,18 +461,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4969,6 +4969,90 @@
     </row>
   </sheetData>
   <mergeCells count="100">
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="B73:B76"/>
+    <mergeCell ref="C73:J73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="G75:H75"/>
+    <mergeCell ref="G74:H74"/>
+    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="C56:J56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="O40:P40"/>
+    <mergeCell ref="Q40:R40"/>
+    <mergeCell ref="S40:T40"/>
+    <mergeCell ref="L39:L42"/>
+    <mergeCell ref="M39:T39"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="O41:P41"/>
+    <mergeCell ref="Q41:R41"/>
+    <mergeCell ref="S41:T41"/>
+    <mergeCell ref="L5:L8"/>
+    <mergeCell ref="M5:T5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="L22:L25"/>
+    <mergeCell ref="M22:T22"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="L73:L76"/>
+    <mergeCell ref="M73:T73"/>
+    <mergeCell ref="M74:N74"/>
+    <mergeCell ref="O74:P74"/>
+    <mergeCell ref="Q74:R74"/>
+    <mergeCell ref="S74:T74"/>
+    <mergeCell ref="M75:N75"/>
+    <mergeCell ref="O75:P75"/>
+    <mergeCell ref="Q75:R75"/>
+    <mergeCell ref="S75:T75"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="M58:N58"/>
+    <mergeCell ref="O58:P58"/>
+    <mergeCell ref="L56:L59"/>
+    <mergeCell ref="M56:T56"/>
+    <mergeCell ref="M57:N57"/>
+    <mergeCell ref="O57:P57"/>
+    <mergeCell ref="Q57:R57"/>
+    <mergeCell ref="S57:T57"/>
+    <mergeCell ref="Q58:R58"/>
+    <mergeCell ref="S58:T58"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="I74:J74"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:J22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="B39:B42"/>
@@ -4985,90 +5069,6 @@
     <mergeCell ref="G24:H24"/>
     <mergeCell ref="I24:J24"/>
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="I74:J74"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:J22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="M58:N58"/>
-    <mergeCell ref="O58:P58"/>
-    <mergeCell ref="L56:L59"/>
-    <mergeCell ref="M56:T56"/>
-    <mergeCell ref="M57:N57"/>
-    <mergeCell ref="O57:P57"/>
-    <mergeCell ref="Q57:R57"/>
-    <mergeCell ref="S57:T57"/>
-    <mergeCell ref="Q58:R58"/>
-    <mergeCell ref="S58:T58"/>
-    <mergeCell ref="L73:L76"/>
-    <mergeCell ref="M73:T73"/>
-    <mergeCell ref="M74:N74"/>
-    <mergeCell ref="O74:P74"/>
-    <mergeCell ref="Q74:R74"/>
-    <mergeCell ref="S74:T74"/>
-    <mergeCell ref="M75:N75"/>
-    <mergeCell ref="O75:P75"/>
-    <mergeCell ref="Q75:R75"/>
-    <mergeCell ref="S75:T75"/>
-    <mergeCell ref="L22:L25"/>
-    <mergeCell ref="M22:T22"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="L5:L8"/>
-    <mergeCell ref="M5:T5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="O40:P40"/>
-    <mergeCell ref="Q40:R40"/>
-    <mergeCell ref="S40:T40"/>
-    <mergeCell ref="L39:L42"/>
-    <mergeCell ref="M39:T39"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="O41:P41"/>
-    <mergeCell ref="Q41:R41"/>
-    <mergeCell ref="S41:T41"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="B73:B76"/>
-    <mergeCell ref="C73:J73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="G75:H75"/>
-    <mergeCell ref="G74:H74"/>
-    <mergeCell ref="E75:F75"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="C56:J56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="I57:J57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6276,16 +6276,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="S29:T29"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="M29:N29"/>
     <mergeCell ref="K29:L29"/>
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="B24:B25"/>
@@ -6302,6 +6292,16 @@
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B6:B7"/>
+    <mergeCell ref="U29:V29"/>
+    <mergeCell ref="S29:T29"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="B29:B30"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6344,71 +6344,71 @@
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="38"/>
-      <c r="R3" s="38"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="32"/>
       <c r="S3" s="11"/>
       <c r="T3" s="11"/>
       <c r="U3" s="11"/>
       <c r="V3" s="11"/>
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B4" s="36"/>
-      <c r="C4" s="35" t="s">
+      <c r="B4" s="33"/>
+      <c r="C4" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36" t="s">
+      <c r="D4" s="33"/>
+      <c r="E4" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="36"/>
-      <c r="G4" s="31" t="s">
+      <c r="F4" s="33"/>
+      <c r="G4" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="32"/>
-      <c r="I4" s="31" t="s">
+      <c r="H4" s="36"/>
+      <c r="I4" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="32"/>
-      <c r="K4" s="31" t="s">
+      <c r="J4" s="36"/>
+      <c r="K4" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="L4" s="32"/>
-      <c r="M4" s="31" t="s">
+      <c r="L4" s="36"/>
+      <c r="M4" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="N4" s="32"/>
-      <c r="O4" s="31" t="s">
+      <c r="N4" s="36"/>
+      <c r="O4" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="31" t="s">
+      <c r="P4" s="36"/>
+      <c r="Q4" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="R4" s="32"/>
-      <c r="S4" s="31" t="s">
+      <c r="R4" s="36"/>
+      <c r="S4" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="T4" s="32"/>
-      <c r="U4" s="31" t="s">
+      <c r="T4" s="36"/>
+      <c r="U4" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="V4" s="32"/>
+      <c r="V4" s="36"/>
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B5" s="36"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="12" t="s">
         <v>6</v>
       </c>
@@ -7246,71 +7246,71 @@
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
-      <c r="F26" s="37" t="s">
+      <c r="F26" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="38"/>
-      <c r="J26" s="38"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="38"/>
-      <c r="M26" s="38"/>
-      <c r="N26" s="38"/>
-      <c r="O26" s="38"/>
-      <c r="P26" s="38"/>
-      <c r="Q26" s="38"/>
-      <c r="R26" s="38"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="32"/>
+      <c r="P26" s="32"/>
+      <c r="Q26" s="32"/>
+      <c r="R26" s="32"/>
       <c r="S26" s="11"/>
       <c r="T26" s="11"/>
       <c r="U26" s="11"/>
       <c r="V26" s="11"/>
     </row>
     <row r="27" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B27" s="36"/>
-      <c r="C27" s="35" t="s">
+      <c r="B27" s="33"/>
+      <c r="C27" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36" t="s">
+      <c r="D27" s="33"/>
+      <c r="E27" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="F27" s="36"/>
-      <c r="G27" s="31" t="s">
+      <c r="F27" s="33"/>
+      <c r="G27" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="H27" s="32"/>
-      <c r="I27" s="31" t="s">
+      <c r="H27" s="36"/>
+      <c r="I27" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="J27" s="32"/>
-      <c r="K27" s="31" t="s">
+      <c r="J27" s="36"/>
+      <c r="K27" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="L27" s="32"/>
-      <c r="M27" s="31" t="s">
+      <c r="L27" s="36"/>
+      <c r="M27" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="N27" s="32"/>
-      <c r="O27" s="31" t="s">
+      <c r="N27" s="36"/>
+      <c r="O27" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="P27" s="32"/>
-      <c r="Q27" s="31" t="s">
+      <c r="P27" s="36"/>
+      <c r="Q27" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="R27" s="32"/>
-      <c r="S27" s="31" t="s">
+      <c r="R27" s="36"/>
+      <c r="S27" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="T27" s="32"/>
-      <c r="U27" s="31" t="s">
+      <c r="T27" s="36"/>
+      <c r="U27" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="V27" s="32"/>
+      <c r="V27" s="36"/>
     </row>
     <row r="28" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B28" s="36"/>
+      <c r="B28" s="33"/>
       <c r="C28" s="12" t="s">
         <v>6</v>
       </c>
@@ -8308,40 +8308,40 @@
       </c>
     </row>
     <row r="43" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="D43" s="33" t="s">
+      <c r="D43" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="E43" s="34"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="34"/>
-      <c r="H43" s="34"/>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="38"/>
     </row>
     <row r="44" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B44" s="35" t="s">
+      <c r="B44" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="35" t="s">
+      <c r="C44" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36" t="s">
+      <c r="D44" s="33"/>
+      <c r="E44" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="F44" s="36"/>
-      <c r="G44" s="31" t="s">
+      <c r="F44" s="33"/>
+      <c r="G44" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="H44" s="32"/>
-      <c r="I44" s="31" t="s">
+      <c r="H44" s="36"/>
+      <c r="I44" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="J44" s="32"/>
-      <c r="K44" s="31" t="s">
+      <c r="J44" s="36"/>
+      <c r="K44" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="L44" s="32"/>
+      <c r="L44" s="36"/>
       <c r="O44" s="17"/>
       <c r="P44" s="17"/>
       <c r="Q44" s="17"/>
@@ -8353,7 +8353,7 @@
       <c r="W44" s="17"/>
     </row>
     <row r="45" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B45" s="35"/>
+      <c r="B45" s="34"/>
       <c r="C45" s="12" t="s">
         <v>6</v>
       </c>
@@ -8971,43 +8971,43 @@
       </c>
     </row>
     <row r="60" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="D60" s="33" t="s">
+      <c r="D60" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="E60" s="34"/>
-      <c r="F60" s="34"/>
-      <c r="G60" s="34"/>
-      <c r="H60" s="34"/>
-      <c r="I60" s="34"/>
-      <c r="J60" s="34"/>
+      <c r="E60" s="38"/>
+      <c r="F60" s="38"/>
+      <c r="G60" s="38"/>
+      <c r="H60" s="38"/>
+      <c r="I60" s="38"/>
+      <c r="J60" s="38"/>
     </row>
     <row r="61" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B61" s="35" t="s">
+      <c r="B61" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C61" s="35" t="s">
+      <c r="C61" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="D61" s="36"/>
-      <c r="E61" s="35" t="s">
+      <c r="D61" s="33"/>
+      <c r="E61" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="F61" s="36"/>
-      <c r="G61" s="35" t="s">
+      <c r="F61" s="33"/>
+      <c r="G61" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="H61" s="36"/>
-      <c r="I61" s="35" t="s">
+      <c r="H61" s="33"/>
+      <c r="I61" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="J61" s="36"/>
-      <c r="K61" s="31" t="s">
+      <c r="J61" s="33"/>
+      <c r="K61" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="L61" s="32"/>
+      <c r="L61" s="36"/>
     </row>
     <row r="62" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B62" s="35"/>
+      <c r="B62" s="34"/>
       <c r="C62" s="12" t="s">
         <v>6</v>
       </c>
@@ -9536,30 +9536,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="F3:R3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="S27:T27"/>
-    <mergeCell ref="U27:V27"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="F26:R26"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="M27:N27"/>
     <mergeCell ref="K61:L61"/>
     <mergeCell ref="D43:J43"/>
     <mergeCell ref="D60:J60"/>
@@ -9574,6 +9550,30 @@
     <mergeCell ref="G44:H44"/>
     <mergeCell ref="I44:J44"/>
     <mergeCell ref="K44:L44"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="S27:T27"/>
+    <mergeCell ref="U27:V27"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="F26:R26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="F3:R3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:R4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12202,6 +12202,30 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="N65:O65"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="Q65:R65"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="Q49:R49"/>
+    <mergeCell ref="N49:O49"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B50:C50"/>
     <mergeCell ref="T33:U33"/>
     <mergeCell ref="T49:U49"/>
     <mergeCell ref="T17:U17"/>
@@ -12212,30 +12236,6 @@
     <mergeCell ref="Q17:R17"/>
     <mergeCell ref="Q33:R33"/>
     <mergeCell ref="N33:O33"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="H66:I66"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="Q65:R65"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="Q49:R49"/>
-    <mergeCell ref="N49:O49"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="N65:O65"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12246,7 +12246,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F629120-A968-46FA-806F-80DB4F7E279A}">
   <dimension ref="B2:V15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
@@ -12907,71 +12907,71 @@
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
       <c r="R1" s="11"/>
       <c r="S1" s="11"/>
       <c r="T1" s="11"/>
       <c r="U1" s="11"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
-      <c r="B2" s="35" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="31" t="s">
+      <c r="E2" s="33"/>
+      <c r="F2" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="32"/>
-      <c r="H2" s="31" t="s">
+      <c r="G2" s="36"/>
+      <c r="H2" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="32"/>
-      <c r="J2" s="31" t="s">
+      <c r="I2" s="36"/>
+      <c r="J2" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="31" t="s">
+      <c r="K2" s="36"/>
+      <c r="L2" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="32"/>
-      <c r="N2" s="31" t="s">
+      <c r="M2" s="36"/>
+      <c r="N2" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="32"/>
-      <c r="P2" s="31" t="s">
+      <c r="O2" s="36"/>
+      <c r="P2" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="31" t="s">
+      <c r="Q2" s="36"/>
+      <c r="R2" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="S2" s="32"/>
-      <c r="T2" s="31" t="s">
+      <c r="S2" s="36"/>
+      <c r="T2" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="U2" s="32"/>
+      <c r="U2" s="36"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="36"/>
+      <c r="A3" s="33"/>
       <c r="B3" s="12" t="s">
         <v>6</v>
       </c>
@@ -13788,10 +13788,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6187A48A-D5CA-46DB-A520-3F1A66BE5931}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80C7930F-A427-4174-8C87-0E5A1BD99A13}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>